<commit_message>
ANTES DE VARIABLE ANCLA
</commit_message>
<xml_diff>
--- a/Indc WDI_V6.xlsx
+++ b/Indc WDI_V6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\messi\OneDrive\Escritorio\escuela\Servicio Social\Python\PCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E8B7BE-D6EA-43EF-84A3-146F51BB8073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787244A7-7F0A-470F-B5E5-D551E4F2C9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="4" xr2:uid="{D86699F4-EEE8-4FD6-B0D7-CE6A5D28E5C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D86699F4-EEE8-4FD6-B0D7-CE6A5D28E5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP growth (annual %)" sheetId="25" r:id="rId1"/>
@@ -554,8 +554,8 @@
   </sheetPr>
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3186,7 +3186,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3298,6 +3298,14 @@
         <f>L2</f>
         <v>4568.56640625</v>
       </c>
+      <c r="V2" s="5">
+        <f>L2</f>
+        <v>4568.56640625</v>
+      </c>
+      <c r="W2" s="5">
+        <f>L2</f>
+        <v>4568.56640625</v>
+      </c>
       <c r="X2" s="5">
         <f>L2</f>
         <v>4568.56640625</v>
@@ -3484,6 +3492,10 @@
       <c r="U5">
         <v>5561.72998046875</v>
       </c>
+      <c r="V5" s="5">
+        <f>U5</f>
+        <v>5561.72998046875</v>
+      </c>
       <c r="W5">
         <v>6021.3984375</v>
       </c>
@@ -4245,6 +4257,10 @@
       <c r="V16">
         <v>259.26324462890602</v>
       </c>
+      <c r="W16" s="5">
+        <f>V16</f>
+        <v>259.26324462890602</v>
+      </c>
       <c r="X16" s="5">
         <f>V16</f>
         <v>259.26324462890602</v>
@@ -4284,6 +4300,10 @@
         <v>387.17062377929699</v>
       </c>
       <c r="V17">
+        <v>395.34167480468801</v>
+      </c>
+      <c r="W17" s="5">
+        <f>V17</f>
         <v>395.34167480468801</v>
       </c>
       <c r="X17" s="5">
@@ -5552,8 +5572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D64FC8F-D734-42A8-9038-CF327D7C7E20}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5673,6 +5693,10 @@
       <c r="U2">
         <v>1.82570004463196</v>
       </c>
+      <c r="V2" s="5">
+        <f>W2</f>
+        <v>1.8550900220871001</v>
+      </c>
       <c r="W2">
         <v>1.8550900220871001</v>
       </c>
@@ -5862,6 +5886,10 @@
       <c r="U5">
         <v>3.1967999935150102</v>
       </c>
+      <c r="V5" s="5">
+        <f>W5</f>
+        <v>3.3064498901367201</v>
+      </c>
       <c r="W5">
         <v>3.3064498901367201</v>
       </c>
@@ -6673,6 +6701,10 @@
       <c r="V16">
         <v>0.645579993724823</v>
       </c>
+      <c r="W16" s="5">
+        <f>V16</f>
+        <v>0.645579993724823</v>
+      </c>
       <c r="X16" s="5">
         <v>0.63812401294708199</v>
       </c>
@@ -6712,6 +6744,10 @@
         <v>0.27129000425338701</v>
       </c>
       <c r="V17">
+        <v>0.28068000078201299</v>
+      </c>
+      <c r="W17" s="5">
+        <f>V17</f>
         <v>0.28068000078201299</v>
       </c>
       <c r="X17" s="5">
@@ -13144,8 +13180,8 @@
   </sheetPr>
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15780,7 +15816,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18410,8 +18446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3688E331-455B-4BA0-BB0B-12E4157B96E2}">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18534,6 +18570,14 @@
       <c r="U2" s="5">
         <v>12.7</v>
       </c>
+      <c r="V2" s="5">
+        <f>U2</f>
+        <v>12.7</v>
+      </c>
+      <c r="W2" s="5">
+        <f>T2</f>
+        <v>12.7</v>
+      </c>
       <c r="X2" s="5">
         <f>T2</f>
         <v>12.7</v>
@@ -18672,6 +18716,14 @@
       <c r="U4">
         <v>12.5</v>
       </c>
+      <c r="V4" s="5">
+        <f>U4</f>
+        <v>12.5</v>
+      </c>
+      <c r="W4" s="5">
+        <f>U4</f>
+        <v>12.5</v>
+      </c>
       <c r="X4" s="5">
         <f>U4</f>
         <v>12.5</v>
@@ -18735,6 +18787,10 @@
       <c r="V5">
         <v>11.7</v>
       </c>
+      <c r="W5" s="5">
+        <f>V5</f>
+        <v>11.7</v>
+      </c>
       <c r="X5" s="5">
         <f>V5</f>
         <v>11.7</v>
@@ -18938,6 +18994,10 @@
       <c r="V8">
         <v>12</v>
       </c>
+      <c r="W8" s="5">
+        <f>V8</f>
+        <v>12</v>
+      </c>
       <c r="X8" s="5">
         <f>V8</f>
         <v>12</v>
@@ -19727,6 +19787,14 @@
         <f>O20</f>
         <v>11</v>
       </c>
+      <c r="V20" s="5">
+        <f>U20</f>
+        <v>11</v>
+      </c>
+      <c r="W20" s="5">
+        <f>V20</f>
+        <v>11</v>
+      </c>
       <c r="X20" s="5">
         <f>O20</f>
         <v>11</v>
@@ -20037,6 +20105,10 @@
       <c r="V25">
         <v>24.7</v>
       </c>
+      <c r="W25" s="5">
+        <f>V25</f>
+        <v>24.7</v>
+      </c>
       <c r="X25">
         <v>22.5</v>
       </c>
@@ -20164,6 +20236,14 @@
         <v>9</v>
       </c>
       <c r="U27">
+        <v>9.4</v>
+      </c>
+      <c r="V27" s="5">
+        <f>U27</f>
+        <v>9.4</v>
+      </c>
+      <c r="W27" s="5">
+        <f>V27</f>
         <v>9.4</v>
       </c>
       <c r="X27" s="5">
@@ -20731,8 +20811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E5E40-226B-4325-B9E0-4ECCDE7D7349}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20852,6 +20932,14 @@
         <f>T2</f>
         <v>1</v>
       </c>
+      <c r="V2" s="5">
+        <f>U2</f>
+        <v>1</v>
+      </c>
+      <c r="W2" s="5">
+        <f>T2</f>
+        <v>1</v>
+      </c>
       <c r="X2" s="5">
         <f>T2</f>
         <v>1</v>
@@ -20990,6 +21078,14 @@
       <c r="U4">
         <v>0.7</v>
       </c>
+      <c r="V4" s="5">
+        <f>U4</f>
+        <v>0.7</v>
+      </c>
+      <c r="W4" s="5">
+        <f>U4</f>
+        <v>0.7</v>
+      </c>
       <c r="X4" s="5">
         <f>U4</f>
         <v>0.7</v>
@@ -21053,6 +21149,10 @@
       <c r="V5">
         <v>0.1</v>
       </c>
+      <c r="W5" s="5">
+        <f>V5</f>
+        <v>0.1</v>
+      </c>
       <c r="X5" s="5">
         <f>V5</f>
         <v>0.1</v>
@@ -21257,6 +21357,10 @@
       <c r="V8">
         <v>0.5</v>
       </c>
+      <c r="W8" s="5">
+        <f>V8</f>
+        <v>0.5</v>
+      </c>
       <c r="X8" s="5">
         <f>V8</f>
         <v>0.5</v>
@@ -22047,6 +22151,14 @@
         <f>O20</f>
         <v>1.4</v>
       </c>
+      <c r="V20" s="5">
+        <f>O20</f>
+        <v>1.4</v>
+      </c>
+      <c r="W20" s="5">
+        <f>O20</f>
+        <v>1.4</v>
+      </c>
       <c r="X20" s="5">
         <f>O20</f>
         <v>1.4</v>
@@ -22359,6 +22471,10 @@
       <c r="V25">
         <v>30.3</v>
       </c>
+      <c r="W25" s="5">
+        <f>V25</f>
+        <v>30.3</v>
+      </c>
       <c r="X25">
         <v>21.8</v>
       </c>
@@ -22486,6 +22602,14 @@
         <v>0.5</v>
       </c>
       <c r="U27">
+        <v>0.5</v>
+      </c>
+      <c r="V27" s="5">
+        <f>U27</f>
+        <v>0.5</v>
+      </c>
+      <c r="W27" s="5">
+        <f>U27</f>
         <v>0.5</v>
       </c>
       <c r="X27" s="5">
@@ -22958,8 +23082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E209C58E-6D7E-40CA-9A2E-E09184173097}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25410,7 +25534,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28008,7 +28132,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30361,7 +30485,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Final código, para datos socioeconómicos
</commit_message>
<xml_diff>
--- a/Indc WDI_V6.xlsx
+++ b/Indc WDI_V6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\messi\OneDrive\Escritorio\escuela\Servicio Social\Python\PCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787244A7-7F0A-470F-B5E5-D551E4F2C9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5930168-847C-45C0-82F9-F20211756350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D86699F4-EEE8-4FD6-B0D7-CE6A5D28E5C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="6" xr2:uid="{D86699F4-EEE8-4FD6-B0D7-CE6A5D28E5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP growth (annual %)" sheetId="25" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="37">
   <si>
     <t>KOR</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t>IND</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>MYS</t>
+  </si>
+  <si>
+    <t>THA</t>
+  </si>
+  <si>
+    <t>VNM</t>
   </si>
 </sst>
 </file>
@@ -552,10 +564,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="I7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z35" sqref="Z35:Z42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3176,6 +3188,314 @@
         <v>2.8875560090601602</v>
       </c>
     </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>4.3416341791447497</v>
+      </c>
+      <c r="C35">
+        <v>2.5727803861407801</v>
+      </c>
+      <c r="D35">
+        <v>1.79566077025204</v>
+      </c>
+      <c r="E35">
+        <v>3.1523465382741902</v>
+      </c>
+      <c r="F35">
+        <v>2.45790441131264</v>
+      </c>
+      <c r="G35">
+        <v>2.73266076130363</v>
+      </c>
+      <c r="H35">
+        <v>2.3806940248706598</v>
+      </c>
+      <c r="I35">
+        <v>2.6248800197125099</v>
+      </c>
+      <c r="J35">
+        <v>-0.24879729813224599</v>
+      </c>
+      <c r="K35">
+        <v>-4.6205537195686004</v>
+      </c>
+      <c r="L35">
+        <v>2.2333151263108002</v>
+      </c>
+      <c r="M35">
+        <v>1.1383623474489299</v>
+      </c>
+      <c r="N35">
+        <v>1.5089983744101401</v>
+      </c>
+      <c r="O35">
+        <v>1.7999214936266299</v>
+      </c>
+      <c r="P35">
+        <v>3.1946373128020999</v>
+      </c>
+      <c r="Q35">
+        <v>2.2228884490843699</v>
+      </c>
+      <c r="R35">
+        <v>1.92171007763831</v>
+      </c>
+      <c r="S35">
+        <v>2.6565048930997199</v>
+      </c>
+      <c r="T35">
+        <v>1.40519026609273</v>
+      </c>
+      <c r="U35">
+        <v>1.62447515947532</v>
+      </c>
+      <c r="V35">
+        <v>-10.296918873756701</v>
+      </c>
+      <c r="W35">
+        <v>8.5759509048564997</v>
+      </c>
+      <c r="X35">
+        <v>4.8390851471440302</v>
+      </c>
+      <c r="Y35">
+        <v>0.33996615800346303</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>8.85886816969386</v>
+      </c>
+      <c r="C36">
+        <v>0.51767531919286103</v>
+      </c>
+      <c r="D36">
+        <v>5.3909883069279703</v>
+      </c>
+      <c r="E36">
+        <v>5.7884992858875002</v>
+      </c>
+      <c r="F36">
+        <v>6.7834377237030496</v>
+      </c>
+      <c r="G36">
+        <v>5.3321391614148599</v>
+      </c>
+      <c r="H36">
+        <v>5.5848470671515003</v>
+      </c>
+      <c r="I36">
+        <v>6.2987859274094697</v>
+      </c>
+      <c r="J36">
+        <v>4.8317698891309702</v>
+      </c>
+      <c r="K36">
+        <v>-1.51352871598714</v>
+      </c>
+      <c r="L36">
+        <v>7.4248473832609703</v>
+      </c>
+      <c r="M36">
+        <v>5.2939128341400297</v>
+      </c>
+      <c r="N36">
+        <v>5.4734541925385303</v>
+      </c>
+      <c r="O36">
+        <v>4.6937225255789299</v>
+      </c>
+      <c r="P36">
+        <v>6.0067219455820302</v>
+      </c>
+      <c r="Q36">
+        <v>5.0915324215501103</v>
+      </c>
+      <c r="R36">
+        <v>4.4497813976154097</v>
+      </c>
+      <c r="S36">
+        <v>5.8127224098332801</v>
+      </c>
+      <c r="T36">
+        <v>4.8430869763488102</v>
+      </c>
+      <c r="U36">
+        <v>4.4131874212958602</v>
+      </c>
+      <c r="V36">
+        <v>-5.4568465842670104</v>
+      </c>
+      <c r="W36">
+        <v>3.31534954399166</v>
+      </c>
+      <c r="X36">
+        <v>8.8618218757804605</v>
+      </c>
+      <c r="Y36">
+        <v>3.5554871541050899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>4.4552470433501403</v>
+      </c>
+      <c r="C37">
+        <v>3.4442490096837202</v>
+      </c>
+      <c r="D37">
+        <v>6.1490360521003602</v>
+      </c>
+      <c r="E37">
+        <v>7.1892433034097101</v>
+      </c>
+      <c r="F37">
+        <v>6.2893421428579499</v>
+      </c>
+      <c r="G37">
+        <v>4.1876384288433703</v>
+      </c>
+      <c r="H37">
+        <v>4.9678108924610704</v>
+      </c>
+      <c r="I37">
+        <v>5.4351516905080901</v>
+      </c>
+      <c r="J37">
+        <v>1.72569884866334</v>
+      </c>
+      <c r="K37">
+        <v>-0.69061823230057895</v>
+      </c>
+      <c r="L37">
+        <v>7.5133905326162402</v>
+      </c>
+      <c r="M37">
+        <v>0.84013208305333398</v>
+      </c>
+      <c r="N37">
+        <v>7.2427962024964199</v>
+      </c>
+      <c r="O37">
+        <v>2.6874955632055602</v>
+      </c>
+      <c r="P37">
+        <v>0.98446886361942598</v>
+      </c>
+      <c r="Q37">
+        <v>3.13404724911635</v>
+      </c>
+      <c r="R37">
+        <v>3.4351577169218199</v>
+      </c>
+      <c r="S37">
+        <v>4.1776810321001001</v>
+      </c>
+      <c r="T37">
+        <v>4.2228702874607098</v>
+      </c>
+      <c r="U37">
+        <v>2.1145577962827802</v>
+      </c>
+      <c r="V37">
+        <v>-6.0500384685162203</v>
+      </c>
+      <c r="W37">
+        <v>1.5681817650118599</v>
+      </c>
+      <c r="X37">
+        <v>2.4627693405035598</v>
+      </c>
+      <c r="Y37">
+        <v>1.8872572505093399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>6.7873164046315102</v>
+      </c>
+      <c r="C38">
+        <v>6.1928933123337702</v>
+      </c>
+      <c r="D38">
+        <v>6.32082099160833</v>
+      </c>
+      <c r="E38">
+        <v>6.8990634905525798</v>
+      </c>
+      <c r="F38">
+        <v>7.5364106089038598</v>
+      </c>
+      <c r="G38">
+        <v>7.5472477289591797</v>
+      </c>
+      <c r="H38">
+        <v>6.9779548105671099</v>
+      </c>
+      <c r="I38">
+        <v>7.1295044860543904</v>
+      </c>
+      <c r="J38">
+        <v>5.6617712089136196</v>
+      </c>
+      <c r="K38">
+        <v>5.3978975401418099</v>
+      </c>
+      <c r="L38">
+        <v>6.4232448223948202</v>
+      </c>
+      <c r="M38">
+        <v>6.4131688968168303</v>
+      </c>
+      <c r="N38">
+        <v>5.5045447041189002</v>
+      </c>
+      <c r="O38">
+        <v>5.55351081026072</v>
+      </c>
+      <c r="P38">
+        <v>6.4222431211856703</v>
+      </c>
+      <c r="Q38">
+        <v>6.9871543059861096</v>
+      </c>
+      <c r="R38">
+        <v>6.6900089266042402</v>
+      </c>
+      <c r="S38">
+        <v>6.9401903735920598</v>
+      </c>
+      <c r="T38">
+        <v>7.46500685572751</v>
+      </c>
+      <c r="U38">
+        <v>7.35926270105006</v>
+      </c>
+      <c r="V38">
+        <v>2.8654132091227198</v>
+      </c>
+      <c r="W38">
+        <v>2.5537285264813101</v>
+      </c>
+      <c r="X38">
+        <v>8.1235144676734308</v>
+      </c>
+      <c r="Y38">
+        <v>5.0464307361882002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3183,10 +3503,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1076E55-44ED-47AE-BB7E-A9F420480294}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5563,6 +5883,244 @@
         <v>4825.18017578125</v>
       </c>
     </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>2893.37573242188</v>
+      </c>
+      <c r="C35">
+        <v>3078.40942382812</v>
+      </c>
+      <c r="D35">
+        <v>3335.62719726562</v>
+      </c>
+      <c r="E35">
+        <v>3631.25708007812</v>
+      </c>
+      <c r="F35">
+        <v>3818.2353515625</v>
+      </c>
+      <c r="G35">
+        <v>4117.7451171875</v>
+      </c>
+      <c r="H35">
+        <v>4176.4375</v>
+      </c>
+      <c r="I35">
+        <v>4122.71337890625</v>
+      </c>
+      <c r="J35">
+        <v>4077.28662109375</v>
+      </c>
+      <c r="K35">
+        <v>4113.41552734375</v>
+      </c>
+      <c r="L35">
+        <v>4089.20556640625</v>
+      </c>
+      <c r="M35">
+        <v>3973.02368164062</v>
+      </c>
+      <c r="N35">
+        <v>4017.98193359375</v>
+      </c>
+      <c r="O35">
+        <v>4171.8076171875</v>
+      </c>
+      <c r="P35">
+        <v>4280.7998046875</v>
+      </c>
+      <c r="Q35">
+        <v>4389.5625</v>
+      </c>
+      <c r="R35">
+        <v>4434.6591796875</v>
+      </c>
+      <c r="S35">
+        <v>4472.6943359375</v>
+      </c>
+      <c r="U35" s="5">
+        <f>S35</f>
+        <v>4472.6943359375</v>
+      </c>
+      <c r="V35" s="5">
+        <f>S35</f>
+        <v>4472.6943359375</v>
+      </c>
+      <c r="W35" s="5">
+        <f>S35</f>
+        <v>4472.6943359375</v>
+      </c>
+      <c r="X35" s="5">
+        <f>S35</f>
+        <v>4472.6943359375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>282.98355102539102</v>
+      </c>
+      <c r="D36">
+        <v>300.560791015625</v>
+      </c>
+      <c r="F36">
+        <v>507.42810058593801</v>
+      </c>
+      <c r="H36">
+        <v>371.05001831054699</v>
+      </c>
+      <c r="I36" s="5">
+        <f>J36</f>
+        <v>598.97222900390602</v>
+      </c>
+      <c r="J36">
+        <v>598.97222900390602</v>
+      </c>
+      <c r="K36">
+        <v>1063.03527832031</v>
+      </c>
+      <c r="L36">
+        <v>1452.73364257812</v>
+      </c>
+      <c r="M36">
+        <v>1633.85559082031</v>
+      </c>
+      <c r="N36">
+        <v>1769.90747070312</v>
+      </c>
+      <c r="P36">
+        <v>2015.97277832031</v>
+      </c>
+      <c r="Q36">
+        <v>2256.60229492188</v>
+      </c>
+      <c r="R36">
+        <v>2334.07983398438</v>
+      </c>
+      <c r="T36">
+        <v>2110.44311523438</v>
+      </c>
+      <c r="U36" s="5">
+        <f>T36</f>
+        <v>2110.44311523438</v>
+      </c>
+      <c r="V36">
+        <v>711.51037597656205</v>
+      </c>
+      <c r="W36" s="5">
+        <f>V36</f>
+        <v>711.51037597656205</v>
+      </c>
+      <c r="X36" s="5">
+        <f>V36</f>
+        <v>711.51037597656205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5">
+        <f>C37</f>
+        <v>279.59954833984398</v>
+      </c>
+      <c r="C37">
+        <v>279.59954833984398</v>
+      </c>
+      <c r="E37">
+        <v>280.52761840820301</v>
+      </c>
+      <c r="G37">
+        <v>311.93078613281199</v>
+      </c>
+      <c r="I37">
+        <v>320.05038452148398</v>
+      </c>
+      <c r="K37">
+        <v>324.12832641601602</v>
+      </c>
+      <c r="L37" s="5">
+        <f>M37</f>
+        <v>528.556884765625</v>
+      </c>
+      <c r="M37">
+        <v>528.556884765625</v>
+      </c>
+      <c r="O37">
+        <v>773.81018066406205</v>
+      </c>
+      <c r="P37">
+        <v>941.80059814453102</v>
+      </c>
+      <c r="Q37">
+        <v>844.08074951171898</v>
+      </c>
+      <c r="R37">
+        <v>1179.07397460938</v>
+      </c>
+      <c r="S37">
+        <v>1315.74987792969</v>
+      </c>
+      <c r="T37">
+        <v>1712.15368652344</v>
+      </c>
+      <c r="U37">
+        <v>1744.16223144531</v>
+      </c>
+      <c r="V37">
+        <v>2018.34790039062</v>
+      </c>
+      <c r="W37">
+        <v>1695.7958984375</v>
+      </c>
+      <c r="X37">
+        <v>1863.07580566406</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <f>D38</f>
+        <v>119.019989013672</v>
+      </c>
+      <c r="D38">
+        <v>119.019989013672</v>
+      </c>
+      <c r="L38" s="5">
+        <f>O38</f>
+        <v>684.84167480468795</v>
+      </c>
+      <c r="O38">
+        <v>684.84167480468795</v>
+      </c>
+      <c r="Q38">
+        <v>681.681640625</v>
+      </c>
+      <c r="S38">
+        <v>707.70007324218795</v>
+      </c>
+      <c r="U38">
+        <v>754.61749267578102</v>
+      </c>
+      <c r="V38" s="5">
+        <f>U38</f>
+        <v>754.61749267578102</v>
+      </c>
+      <c r="W38">
+        <v>767.88665771484398</v>
+      </c>
+      <c r="X38" s="5">
+        <f>W38</f>
+        <v>767.88665771484398</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5570,10 +6128,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D64FC8F-D734-42A8-9038-CF327D7C7E20}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8004,6 +8562,262 @@
       </c>
       <c r="X34">
         <v>3.5862300395965598</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1.60962998867035</v>
+      </c>
+      <c r="C35">
+        <v>1.5954500436782799</v>
+      </c>
+      <c r="D35">
+        <v>1.6138299703598</v>
+      </c>
+      <c r="E35">
+        <v>1.58131003379822</v>
+      </c>
+      <c r="F35">
+        <v>1.53088998794556</v>
+      </c>
+      <c r="G35">
+        <v>1.5500400066375699</v>
+      </c>
+      <c r="H35">
+        <v>1.57625997066498</v>
+      </c>
+      <c r="I35">
+        <v>1.6182999610900899</v>
+      </c>
+      <c r="J35">
+        <v>1.6090099811553999</v>
+      </c>
+      <c r="K35">
+        <v>1.66990995407104</v>
+      </c>
+      <c r="L35">
+        <v>1.63885998725891</v>
+      </c>
+      <c r="M35">
+        <v>1.6468100547790501</v>
+      </c>
+      <c r="N35">
+        <v>1.5758700370788601</v>
+      </c>
+      <c r="O35">
+        <v>1.62095999717712</v>
+      </c>
+      <c r="P35">
+        <v>2.2648799419403098</v>
+      </c>
+      <c r="Q35">
+        <v>2.2756600379943799</v>
+      </c>
+      <c r="R35">
+        <v>2.3205199241638201</v>
+      </c>
+      <c r="S35">
+        <v>2.3260200023651101</v>
+      </c>
+      <c r="T35">
+        <v>2.7112400531768799</v>
+      </c>
+      <c r="U35">
+        <v>2.6707999706268302</v>
+      </c>
+      <c r="V35">
+        <v>2.9388298988342298</v>
+      </c>
+      <c r="W35">
+        <v>2.8971099853515598</v>
+      </c>
+      <c r="X35" s="5">
+        <f>W35</f>
+        <v>2.8971099853515598</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0.468989998102188</v>
+      </c>
+      <c r="D36">
+        <v>0.65254002809524503</v>
+      </c>
+      <c r="F36">
+        <v>0.59990000724792503</v>
+      </c>
+      <c r="H36">
+        <v>0.61106002330779996</v>
+      </c>
+      <c r="I36" s="5">
+        <f>H36</f>
+        <v>0.61106002330779996</v>
+      </c>
+      <c r="J36">
+        <v>0.78846997022628795</v>
+      </c>
+      <c r="K36">
+        <v>1.01001000404358</v>
+      </c>
+      <c r="L36">
+        <v>1.0360800027847299</v>
+      </c>
+      <c r="M36">
+        <v>1.03341996669769</v>
+      </c>
+      <c r="N36">
+        <v>1.09268999099731</v>
+      </c>
+      <c r="P36">
+        <v>1.2627500295639</v>
+      </c>
+      <c r="Q36">
+        <v>1.2794500589370701</v>
+      </c>
+      <c r="R36">
+        <v>1.4151699542999301</v>
+      </c>
+      <c r="T36">
+        <v>1.04025995731354</v>
+      </c>
+      <c r="U36" s="5">
+        <f>T36</f>
+        <v>1.04025995731354</v>
+      </c>
+      <c r="V36">
+        <v>0.95055001974105802</v>
+      </c>
+      <c r="W36" s="5">
+        <f>V36</f>
+        <v>0.95055001974105802</v>
+      </c>
+      <c r="X36" s="5">
+        <f>V36</f>
+        <v>0.95055001974105802</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.244709998369217</v>
+      </c>
+      <c r="C37">
+        <v>0.25231000781059298</v>
+      </c>
+      <c r="D37">
+        <v>0.23055000603199</v>
+      </c>
+      <c r="E37">
+        <v>0.24534000456333199</v>
+      </c>
+      <c r="F37">
+        <v>0.23827999830245999</v>
+      </c>
+      <c r="G37">
+        <v>0.218889996409416</v>
+      </c>
+      <c r="H37">
+        <v>0.23271000385284399</v>
+      </c>
+      <c r="I37">
+        <v>0.200800001621246</v>
+      </c>
+      <c r="J37">
+        <v>0.20330999791622201</v>
+      </c>
+      <c r="K37">
+        <v>0.23454999923706099</v>
+      </c>
+      <c r="L37" s="5">
+        <f>K37</f>
+        <v>0.23454999923706099</v>
+      </c>
+      <c r="M37">
+        <v>0.361460000276566</v>
+      </c>
+      <c r="O37">
+        <v>0.44163998961448703</v>
+      </c>
+      <c r="P37">
+        <v>0.47988000512123102</v>
+      </c>
+      <c r="Q37">
+        <v>0.61608999967575095</v>
+      </c>
+      <c r="R37">
+        <v>0.77828997373580899</v>
+      </c>
+      <c r="S37">
+        <v>1.00165998935699</v>
+      </c>
+      <c r="T37">
+        <v>1.1137399673461901</v>
+      </c>
+      <c r="U37">
+        <v>1.1431699991226201</v>
+      </c>
+      <c r="V37">
+        <v>1.32817995548248</v>
+      </c>
+      <c r="W37">
+        <v>1.2080700397491499</v>
+      </c>
+      <c r="X37">
+        <v>1.159019947052</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <f>D38</f>
+        <v>0.19272999465465501</v>
+      </c>
+      <c r="D38">
+        <v>0.19272999465465501</v>
+      </c>
+      <c r="I38" s="5">
+        <f>D38</f>
+        <v>0.19272999465465501</v>
+      </c>
+      <c r="L38" s="5">
+        <f>M38</f>
+        <v>0.149550005793571</v>
+      </c>
+      <c r="M38">
+        <v>0.149550005793571</v>
+      </c>
+      <c r="O38">
+        <v>0.29932001233100902</v>
+      </c>
+      <c r="Q38">
+        <v>0.356290012598038</v>
+      </c>
+      <c r="S38">
+        <v>0.41894999146461498</v>
+      </c>
+      <c r="U38">
+        <v>0.41651999950408902</v>
+      </c>
+      <c r="V38" s="5">
+        <f>U38</f>
+        <v>0.41651999950408902</v>
+      </c>
+      <c r="W38">
+        <v>0.42493999004364003</v>
+      </c>
+      <c r="X38" s="5">
+        <f>W38</f>
+        <v>0.42493999004364003</v>
       </c>
     </row>
   </sheetData>
@@ -8016,7 +8830,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10644,10 +11458,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575C0386-4DAA-4C42-A1EB-06E5AACD93A5}">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13166,6 +13980,293 @@
       </c>
       <c r="X34">
         <v>4.17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>4.07</v>
+      </c>
+      <c r="C35">
+        <v>3.99</v>
+      </c>
+      <c r="D35">
+        <v>3.87</v>
+      </c>
+      <c r="E35">
+        <v>3.82</v>
+      </c>
+      <c r="F35">
+        <v>3.69</v>
+      </c>
+      <c r="G35">
+        <v>3.61</v>
+      </c>
+      <c r="H35">
+        <v>3.47</v>
+      </c>
+      <c r="I35">
+        <v>3.26</v>
+      </c>
+      <c r="J35">
+        <v>3.22</v>
+      </c>
+      <c r="K35">
+        <v>3.17</v>
+      </c>
+      <c r="L35">
+        <v>3.21</v>
+      </c>
+      <c r="M35">
+        <v>2.94</v>
+      </c>
+      <c r="N35">
+        <v>2.98</v>
+      </c>
+      <c r="O35">
+        <v>2.88</v>
+      </c>
+      <c r="P35">
+        <v>2.63</v>
+      </c>
+      <c r="Q35">
+        <v>2.59</v>
+      </c>
+      <c r="R35">
+        <v>2.5</v>
+      </c>
+      <c r="S35">
+        <v>2.41</v>
+      </c>
+      <c r="T35">
+        <v>2.34</v>
+      </c>
+      <c r="U35">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="V35">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X35">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>5.46</v>
+      </c>
+      <c r="C36">
+        <v>5.65</v>
+      </c>
+      <c r="D36">
+        <v>5.54</v>
+      </c>
+      <c r="E36">
+        <v>5.61</v>
+      </c>
+      <c r="F36">
+        <v>5.66</v>
+      </c>
+      <c r="G36">
+        <v>5.85</v>
+      </c>
+      <c r="H36">
+        <v>5.57</v>
+      </c>
+      <c r="I36">
+        <v>5.59</v>
+      </c>
+      <c r="J36">
+        <v>5.65</v>
+      </c>
+      <c r="K36">
+        <v>5.42</v>
+      </c>
+      <c r="L36">
+        <v>5.23</v>
+      </c>
+      <c r="M36">
+        <v>5.18</v>
+      </c>
+      <c r="N36">
+        <v>4.99</v>
+      </c>
+      <c r="O36">
+        <v>5.38</v>
+      </c>
+      <c r="P36">
+        <v>5.18</v>
+      </c>
+      <c r="Q36">
+        <v>4.72</v>
+      </c>
+      <c r="R36">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="S36">
+        <v>4.28</v>
+      </c>
+      <c r="T36">
+        <v>4.5</v>
+      </c>
+      <c r="U36">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="V36">
+        <v>4.49</v>
+      </c>
+      <c r="W36">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>4.93</v>
+      </c>
+      <c r="C37">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D37">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E37">
+        <v>5.15</v>
+      </c>
+      <c r="F37">
+        <v>5.24</v>
+      </c>
+      <c r="G37">
+        <v>5.18</v>
+      </c>
+      <c r="H37">
+        <v>5.03</v>
+      </c>
+      <c r="I37">
+        <v>4.95</v>
+      </c>
+      <c r="J37">
+        <v>4.99</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+      <c r="L37">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M37">
+        <v>5.05</v>
+      </c>
+      <c r="N37">
+        <v>5.05</v>
+      </c>
+      <c r="O37">
+        <v>5.29</v>
+      </c>
+      <c r="P37">
+        <v>5.22</v>
+      </c>
+      <c r="Q37">
+        <v>5.07</v>
+      </c>
+      <c r="R37">
+        <v>5.04</v>
+      </c>
+      <c r="S37">
+        <v>4.82</v>
+      </c>
+      <c r="T37">
+        <v>4.53</v>
+      </c>
+      <c r="U37">
+        <v>4.53</v>
+      </c>
+      <c r="V37">
+        <v>4.59</v>
+      </c>
+      <c r="W37">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>4.21</v>
+      </c>
+      <c r="C38">
+        <v>4.2</v>
+      </c>
+      <c r="D38">
+        <v>4.28</v>
+      </c>
+      <c r="E38">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F38">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="G38">
+        <v>4.25</v>
+      </c>
+      <c r="H38">
+        <v>4.07</v>
+      </c>
+      <c r="I38">
+        <v>4.09</v>
+      </c>
+      <c r="J38">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="K38">
+        <v>4.29</v>
+      </c>
+      <c r="L38">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="M38">
+        <v>4.18</v>
+      </c>
+      <c r="N38">
+        <v>4.01</v>
+      </c>
+      <c r="O38">
+        <v>3.91</v>
+      </c>
+      <c r="P38">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="Q38">
+        <v>3.54</v>
+      </c>
+      <c r="R38">
+        <v>3.65</v>
+      </c>
+      <c r="S38">
+        <v>3.55</v>
+      </c>
+      <c r="T38">
+        <v>3.9</v>
+      </c>
+      <c r="U38">
+        <v>4.09</v>
+      </c>
+      <c r="V38">
+        <v>4.03</v>
+      </c>
+      <c r="W38">
+        <v>3.85</v>
       </c>
     </row>
   </sheetData>
@@ -13178,10 +14279,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="N25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z35" sqref="Z35:Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15800,6 +16901,314 @@
       </c>
       <c r="Y34">
         <v>74577.506539672293</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>43247.636387345803</v>
+      </c>
+      <c r="C35">
+        <v>44189.854889677801</v>
+      </c>
+      <c r="D35">
+        <v>44793.326072707197</v>
+      </c>
+      <c r="E35">
+        <v>45990.715890991298</v>
+      </c>
+      <c r="F35">
+        <v>46853.792539570102</v>
+      </c>
+      <c r="G35">
+        <v>47804.785256968797</v>
+      </c>
+      <c r="H35">
+        <v>48584.435946901198</v>
+      </c>
+      <c r="I35">
+        <v>49472.985996222997</v>
+      </c>
+      <c r="J35">
+        <v>48963.023157871001</v>
+      </c>
+      <c r="K35">
+        <v>46348.753417533502</v>
+      </c>
+      <c r="L35">
+        <v>47013.882412325402</v>
+      </c>
+      <c r="M35">
+        <v>47178.919900106601</v>
+      </c>
+      <c r="N35">
+        <v>47558.993636203697</v>
+      </c>
+      <c r="O35">
+        <v>48091.846596298899</v>
+      </c>
+      <c r="P35">
+        <v>49264.055374122399</v>
+      </c>
+      <c r="Q35">
+        <v>49961.687628765998</v>
+      </c>
+      <c r="R35">
+        <v>50537.341752810797</v>
+      </c>
+      <c r="S35">
+        <v>51528.604674342401</v>
+      </c>
+      <c r="T35">
+        <v>51937.022697729502</v>
+      </c>
+      <c r="U35">
+        <v>52483.812508839197</v>
+      </c>
+      <c r="V35">
+        <v>46907.713926402801</v>
+      </c>
+      <c r="W35">
+        <v>50972.244587998699</v>
+      </c>
+      <c r="X35">
+        <v>52836.0247301829</v>
+      </c>
+      <c r="Y35">
+        <v>52582.061213859401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>18532.909670622699</v>
+      </c>
+      <c r="C36">
+        <v>18186.441133014599</v>
+      </c>
+      <c r="D36">
+        <v>18708.869487727901</v>
+      </c>
+      <c r="E36">
+        <v>19329.0062757538</v>
+      </c>
+      <c r="F36">
+        <v>20168.506209942501</v>
+      </c>
+      <c r="G36">
+        <v>20767.5857243346</v>
+      </c>
+      <c r="H36">
+        <v>21444.485771502801</v>
+      </c>
+      <c r="I36">
+        <v>22305.118263117001</v>
+      </c>
+      <c r="J36">
+        <v>22898.0027575442</v>
+      </c>
+      <c r="K36">
+        <v>22106.641731180101</v>
+      </c>
+      <c r="L36">
+        <v>23307.969854378502</v>
+      </c>
+      <c r="M36">
+        <v>24115.818120395801</v>
+      </c>
+      <c r="N36">
+        <v>25006.358778153699</v>
+      </c>
+      <c r="O36">
+        <v>25736.3525554142</v>
+      </c>
+      <c r="P36">
+        <v>26818.431728165899</v>
+      </c>
+      <c r="Q36">
+        <v>27699.627886038699</v>
+      </c>
+      <c r="R36">
+        <v>28425.370760941201</v>
+      </c>
+      <c r="S36">
+        <v>29551.545759719698</v>
+      </c>
+      <c r="T36">
+        <v>30459.965533806098</v>
+      </c>
+      <c r="U36">
+        <v>31300.5086554849</v>
+      </c>
+      <c r="V36">
+        <v>29200.452632126999</v>
+      </c>
+      <c r="W36">
+        <v>29822.849183161801</v>
+      </c>
+      <c r="X36">
+        <v>32079.151515748901</v>
+      </c>
+      <c r="Y36">
+        <v>32812.299752533603</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>11622.111667101601</v>
+      </c>
+      <c r="C37">
+        <v>11900.8949342988</v>
+      </c>
+      <c r="D37">
+        <v>12511.738130621199</v>
+      </c>
+      <c r="E37">
+        <v>13286.8323292884</v>
+      </c>
+      <c r="F37">
+        <v>13996.5035765712</v>
+      </c>
+      <c r="G37">
+        <v>14457.740966195999</v>
+      </c>
+      <c r="H37">
+        <v>15050.5253765829</v>
+      </c>
+      <c r="I37">
+        <v>15742.095393990499</v>
+      </c>
+      <c r="J37">
+        <v>15891.2171420249</v>
+      </c>
+      <c r="K37">
+        <v>15665.345949885699</v>
+      </c>
+      <c r="L37">
+        <v>16729.774764714999</v>
+      </c>
+      <c r="M37">
+        <v>16765.751402482299</v>
+      </c>
+      <c r="N37">
+        <v>17869.0021183963</v>
+      </c>
+      <c r="O37">
+        <v>18241.7768708</v>
+      </c>
+      <c r="P37">
+        <v>18323.9627436667</v>
+      </c>
+      <c r="Q37">
+        <v>18811.328452170699</v>
+      </c>
+      <c r="R37">
+        <v>19369.919855894601</v>
+      </c>
+      <c r="S37">
+        <v>20093.963199274</v>
+      </c>
+      <c r="T37">
+        <v>20879.1601782531</v>
+      </c>
+      <c r="U37">
+        <v>21277.082511780001</v>
+      </c>
+      <c r="V37">
+        <v>19956.547351365902</v>
+      </c>
+      <c r="W37">
+        <v>20245.242411127099</v>
+      </c>
+      <c r="X37">
+        <v>20741.5235270511</v>
+      </c>
+      <c r="Y37">
+        <v>21142.664333116201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>4349.2234875146196</v>
+      </c>
+      <c r="C38">
+        <v>4570.26846577385</v>
+      </c>
+      <c r="D38">
+        <v>4809.6215111853498</v>
+      </c>
+      <c r="E38">
+        <v>5090.28990869885</v>
+      </c>
+      <c r="F38">
+        <v>5421.0970282912103</v>
+      </c>
+      <c r="G38">
+        <v>5776.3630445126801</v>
+      </c>
+      <c r="H38">
+        <v>6098.2449543651401</v>
+      </c>
+      <c r="I38">
+        <v>6418.5438140287797</v>
+      </c>
+      <c r="J38">
+        <v>6659.1356143206503</v>
+      </c>
+      <c r="K38">
+        <v>6914.3386358954504</v>
+      </c>
+      <c r="L38">
+        <v>7274.7331069801603</v>
+      </c>
+      <c r="M38">
+        <v>7652.6189567227102</v>
+      </c>
+      <c r="N38">
+        <v>7979.8682892685802</v>
+      </c>
+      <c r="O38">
+        <v>8324.1987125004707</v>
+      </c>
+      <c r="P38">
+        <v>8751.8828063437504</v>
+      </c>
+      <c r="Q38">
+        <v>9248.0239606962205</v>
+      </c>
+      <c r="R38">
+        <v>9743.1882231455002</v>
+      </c>
+      <c r="S38">
+        <v>10290.5487142244</v>
+      </c>
+      <c r="T38">
+        <v>10936.893785955799</v>
+      </c>
+      <c r="U38">
+        <v>11628.613914745099</v>
+      </c>
+      <c r="V38">
+        <v>11851.3965685649</v>
+      </c>
+      <c r="W38">
+        <v>12048.9019935536</v>
+      </c>
+      <c r="X38">
+        <v>12930.2562185687</v>
+      </c>
+      <c r="Y38">
+        <v>13491.879417397</v>
       </c>
     </row>
   </sheetData>
@@ -15813,10 +17222,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18435,6 +19844,314 @@
       </c>
       <c r="Y34">
         <v>2.3826693807721102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>3.9694858348566799</v>
+      </c>
+      <c r="C35">
+        <v>2.17865895350474</v>
+      </c>
+      <c r="D35">
+        <v>1.3656328687566801</v>
+      </c>
+      <c r="E35">
+        <v>2.6731433525175601</v>
+      </c>
+      <c r="F35">
+        <v>1.8766323416763799</v>
+      </c>
+      <c r="G35">
+        <v>2.0297027537216499</v>
+      </c>
+      <c r="H35">
+        <v>1.63090511910372</v>
+      </c>
+      <c r="I35">
+        <v>1.82887797708067</v>
+      </c>
+      <c r="J35">
+        <v>-1.03079049724413</v>
+      </c>
+      <c r="K35">
+        <v>-5.3392735409909404</v>
+      </c>
+      <c r="L35">
+        <v>1.4350526082116599</v>
+      </c>
+      <c r="M35">
+        <v>0.35103990420046199</v>
+      </c>
+      <c r="N35">
+        <v>0.80560075750327098</v>
+      </c>
+      <c r="O35">
+        <v>1.1204041956211199</v>
+      </c>
+      <c r="P35">
+        <v>2.4374376547929999</v>
+      </c>
+      <c r="Q35">
+        <v>1.4161080514903099</v>
+      </c>
+      <c r="R35">
+        <v>1.1521911115616801</v>
+      </c>
+      <c r="S35">
+        <v>1.9614465010448601</v>
+      </c>
+      <c r="T35">
+        <v>0.79260446885429303</v>
+      </c>
+      <c r="U35">
+        <v>1.0527939082916</v>
+      </c>
+      <c r="V35">
+        <v>-10.6244160168382</v>
+      </c>
+      <c r="W35">
+        <v>8.6649515002439603</v>
+      </c>
+      <c r="X35">
+        <v>3.6564607998899401</v>
+      </c>
+      <c r="Y35">
+        <v>-0.480663557904705</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>6.3360361057437897</v>
+      </c>
+      <c r="C36">
+        <v>-1.86947729075297</v>
+      </c>
+      <c r="D36">
+        <v>2.8726255504982601</v>
+      </c>
+      <c r="E36">
+        <v>3.3146673476590101</v>
+      </c>
+      <c r="F36">
+        <v>4.3432131078657399</v>
+      </c>
+      <c r="G36">
+        <v>2.9703712717048498</v>
+      </c>
+      <c r="H36">
+        <v>3.2594065393694902</v>
+      </c>
+      <c r="I36">
+        <v>4.0133044027472797</v>
+      </c>
+      <c r="J36">
+        <v>2.6580647877918899</v>
+      </c>
+      <c r="K36">
+        <v>-3.4560264261626901</v>
+      </c>
+      <c r="L36">
+        <v>5.4342407037972302</v>
+      </c>
+      <c r="M36">
+        <v>3.4659743901529501</v>
+      </c>
+      <c r="N36">
+        <v>3.6927656914312101</v>
+      </c>
+      <c r="O36">
+        <v>2.91923259894287</v>
+      </c>
+      <c r="P36">
+        <v>4.20447757863825</v>
+      </c>
+      <c r="Q36">
+        <v>3.2857855627230101</v>
+      </c>
+      <c r="R36">
+        <v>2.6200455756601602</v>
+      </c>
+      <c r="S36">
+        <v>3.9618656454818502</v>
+      </c>
+      <c r="T36">
+        <v>3.07401779071937</v>
+      </c>
+      <c r="U36">
+        <v>2.7595012238144099</v>
+      </c>
+      <c r="V36">
+        <v>-6.7093351308521996</v>
+      </c>
+      <c r="W36">
+        <v>2.1314619977843101</v>
+      </c>
+      <c r="X36">
+        <v>7.5656833414194304</v>
+      </c>
+      <c r="Y36">
+        <v>2.2854352504452198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>3.2802347951487101</v>
+      </c>
+      <c r="C37">
+        <v>2.3987316176482198</v>
+      </c>
+      <c r="D37">
+        <v>5.1327500973225701</v>
+      </c>
+      <c r="E37">
+        <v>6.1949362316833696</v>
+      </c>
+      <c r="F37">
+        <v>5.3411620595106202</v>
+      </c>
+      <c r="G37">
+        <v>3.2953757851134098</v>
+      </c>
+      <c r="H37">
+        <v>4.1001177969151401</v>
+      </c>
+      <c r="I37">
+        <v>4.5949892120282003</v>
+      </c>
+      <c r="J37">
+        <v>0.94728017015650301</v>
+      </c>
+      <c r="K37">
+        <v>-1.4213586669950899</v>
+      </c>
+      <c r="L37">
+        <v>6.7947992864916698</v>
+      </c>
+      <c r="M37">
+        <v>0.215045559628464</v>
+      </c>
+      <c r="N37">
+        <v>6.58038336266074</v>
+      </c>
+      <c r="O37">
+        <v>2.0861531602812802</v>
+      </c>
+      <c r="P37">
+        <v>0.45053655380589003</v>
+      </c>
+      <c r="Q37">
+        <v>2.65971785318402</v>
+      </c>
+      <c r="R37">
+        <v>2.9694415529671798</v>
+      </c>
+      <c r="S37">
+        <v>3.7379780028308698</v>
+      </c>
+      <c r="T37">
+        <v>3.9076262417335501</v>
+      </c>
+      <c r="U37">
+        <v>1.90583495758329</v>
+      </c>
+      <c r="V37">
+        <v>-6.2063732642059897</v>
+      </c>
+      <c r="W37">
+        <v>1.4466182685728499</v>
+      </c>
+      <c r="X37">
+        <v>2.4513468687893001</v>
+      </c>
+      <c r="Y37">
+        <v>1.9339987515475801</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>5.5879295041075601</v>
+      </c>
+      <c r="C38">
+        <v>5.0824010054619304</v>
+      </c>
+      <c r="D38">
+        <v>5.2371769230622203</v>
+      </c>
+      <c r="E38">
+        <v>5.8355610074673798</v>
+      </c>
+      <c r="F38">
+        <v>6.4987874075118697</v>
+      </c>
+      <c r="G38">
+        <v>6.5533971144111698</v>
+      </c>
+      <c r="H38">
+        <v>5.5723974994652803</v>
+      </c>
+      <c r="I38">
+        <v>5.2523121334174796</v>
+      </c>
+      <c r="J38">
+        <v>3.74838603993047</v>
+      </c>
+      <c r="K38">
+        <v>3.8323745956754198</v>
+      </c>
+      <c r="L38">
+        <v>5.2122768360480798</v>
+      </c>
+      <c r="M38">
+        <v>5.1944977799937</v>
+      </c>
+      <c r="N38">
+        <v>4.27630507146044</v>
+      </c>
+      <c r="O38">
+        <v>4.3149888036992099</v>
+      </c>
+      <c r="P38">
+        <v>5.1378409936445602</v>
+      </c>
+      <c r="Q38">
+        <v>5.6689647854156098</v>
+      </c>
+      <c r="R38">
+        <v>5.35427097241221</v>
+      </c>
+      <c r="S38">
+        <v>5.6178786506313303</v>
+      </c>
+      <c r="T38">
+        <v>6.2809582820196699</v>
+      </c>
+      <c r="U38">
+        <v>6.3246488658190696</v>
+      </c>
+      <c r="V38">
+        <v>1.91581434772165</v>
+      </c>
+      <c r="W38">
+        <v>1.6665160417681899</v>
+      </c>
+      <c r="X38">
+        <v>7.3148094779642703</v>
+      </c>
+      <c r="Y38">
+        <v>4.3434808199842099</v>
       </c>
     </row>
   </sheetData>
@@ -18446,8 +20163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3688E331-455B-4BA0-BB0B-12E4157B96E2}">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20708,28 +22425,252 @@
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B35"/>
-      <c r="I35"/>
-      <c r="L35"/>
-      <c r="U35"/>
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>14.5</v>
+      </c>
+      <c r="C35">
+        <v>14.5</v>
+      </c>
+      <c r="D35">
+        <v>13.7</v>
+      </c>
+      <c r="E35">
+        <v>14</v>
+      </c>
+      <c r="F35">
+        <v>13.7</v>
+      </c>
+      <c r="G35">
+        <v>14.5</v>
+      </c>
+      <c r="H35">
+        <v>14.2</v>
+      </c>
+      <c r="I35">
+        <v>14.5</v>
+      </c>
+      <c r="J35">
+        <v>14.7</v>
+      </c>
+      <c r="K35">
+        <v>14</v>
+      </c>
+      <c r="L35">
+        <v>13.2</v>
+      </c>
+      <c r="M35">
+        <v>13.5</v>
+      </c>
+      <c r="N35">
+        <v>13.2</v>
+      </c>
+      <c r="O35">
+        <v>13.2</v>
+      </c>
+      <c r="P35">
+        <v>13.7</v>
+      </c>
+      <c r="Q35">
+        <v>14</v>
+      </c>
+      <c r="R35">
+        <v>14</v>
+      </c>
+      <c r="S35">
+        <v>14.2</v>
+      </c>
+      <c r="T35">
+        <v>14.5</v>
+      </c>
+      <c r="U35">
+        <v>14.5</v>
+      </c>
+      <c r="V35">
+        <v>13.2</v>
+      </c>
+      <c r="W35">
+        <v>13.2</v>
+      </c>
+      <c r="X35" s="5">
+        <f>W35</f>
+        <v>13.2</v>
+      </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B36"/>
-      <c r="I36"/>
-      <c r="L36"/>
-      <c r="U36"/>
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5">
+        <f>E36</f>
+        <v>26.9</v>
+      </c>
+      <c r="E36">
+        <v>26.9</v>
+      </c>
+      <c r="H36">
+        <v>25.6</v>
+      </c>
+      <c r="I36" s="5">
+        <f>H36</f>
+        <v>25.6</v>
+      </c>
+      <c r="J36">
+        <v>26.2</v>
+      </c>
+      <c r="L36" s="5">
+        <f>M36</f>
+        <v>23.8</v>
+      </c>
+      <c r="M36">
+        <v>23.8</v>
+      </c>
+      <c r="O36">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Q36">
+        <v>20.2</v>
+      </c>
+      <c r="T36">
+        <v>20.5</v>
+      </c>
+      <c r="U36" s="5">
+        <f>T36</f>
+        <v>20.5</v>
+      </c>
+      <c r="V36" s="5">
+        <f>W36</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="W36">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="X36" s="5">
+        <f>W36</f>
+        <v>19.899999999999999</v>
+      </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B37"/>
-      <c r="I37"/>
-      <c r="L37"/>
-      <c r="U37"/>
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>29.5</v>
+      </c>
+      <c r="D37">
+        <v>27.2</v>
+      </c>
+      <c r="F37">
+        <v>26.2</v>
+      </c>
+      <c r="H37">
+        <v>25.4</v>
+      </c>
+      <c r="I37">
+        <v>24</v>
+      </c>
+      <c r="J37">
+        <v>24.1</v>
+      </c>
+      <c r="K37">
+        <v>23.5</v>
+      </c>
+      <c r="L37">
+        <v>21.8</v>
+      </c>
+      <c r="M37">
+        <v>19.3</v>
+      </c>
+      <c r="N37">
+        <v>21.5</v>
+      </c>
+      <c r="O37">
+        <v>19.7</v>
+      </c>
+      <c r="P37">
+        <v>19.5</v>
+      </c>
+      <c r="Q37">
+        <v>18</v>
+      </c>
+      <c r="R37">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="S37">
+        <v>18.7</v>
+      </c>
+      <c r="T37">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="U37">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="V37">
+        <v>18</v>
+      </c>
+      <c r="W37">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="X37" s="5">
+        <f>W37</f>
+        <v>17.100000000000001</v>
+      </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B38"/>
-      <c r="I38"/>
-      <c r="L38"/>
-      <c r="U38"/>
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <f>D38</f>
+        <v>42.8</v>
+      </c>
+      <c r="D38">
+        <v>42.8</v>
+      </c>
+      <c r="F38">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="H38">
+        <v>34.4</v>
+      </c>
+      <c r="I38" s="5">
+        <f>H38</f>
+        <v>34.4</v>
+      </c>
+      <c r="J38">
+        <v>32.5</v>
+      </c>
+      <c r="L38">
+        <v>24.8</v>
+      </c>
+      <c r="N38">
+        <v>24</v>
+      </c>
+      <c r="P38">
+        <v>22.6</v>
+      </c>
+      <c r="R38">
+        <v>21.4</v>
+      </c>
+      <c r="T38">
+        <v>20.7</v>
+      </c>
+      <c r="U38" s="5">
+        <f>T38</f>
+        <v>20.7</v>
+      </c>
+      <c r="V38">
+        <v>20.2</v>
+      </c>
+      <c r="W38" s="5">
+        <f>V38</f>
+        <v>20.2</v>
+      </c>
+      <c r="X38">
+        <v>19.899999999999999</v>
+      </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B39"/>
@@ -20809,10 +22750,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E5E40-226B-4325-B9E0-4ECCDE7D7349}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W36" sqref="W36"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23073,6 +25014,254 @@
         <v>2</v>
       </c>
     </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0.7</v>
+      </c>
+      <c r="C35">
+        <v>0.7</v>
+      </c>
+      <c r="D35">
+        <v>0.7</v>
+      </c>
+      <c r="E35">
+        <v>0.7</v>
+      </c>
+      <c r="F35">
+        <v>0.5</v>
+      </c>
+      <c r="G35">
+        <v>0.7</v>
+      </c>
+      <c r="H35">
+        <v>0.7</v>
+      </c>
+      <c r="I35">
+        <v>0.7</v>
+      </c>
+      <c r="J35">
+        <v>0.7</v>
+      </c>
+      <c r="K35">
+        <v>0.7</v>
+      </c>
+      <c r="L35">
+        <v>0.7</v>
+      </c>
+      <c r="M35">
+        <v>0.7</v>
+      </c>
+      <c r="N35">
+        <v>0.7</v>
+      </c>
+      <c r="O35">
+        <v>0.5</v>
+      </c>
+      <c r="P35">
+        <v>0.5</v>
+      </c>
+      <c r="Q35">
+        <v>0.7</v>
+      </c>
+      <c r="R35">
+        <v>0.7</v>
+      </c>
+      <c r="S35">
+        <v>0.7</v>
+      </c>
+      <c r="T35">
+        <v>0.7</v>
+      </c>
+      <c r="U35">
+        <v>0.7</v>
+      </c>
+      <c r="V35">
+        <v>0.7</v>
+      </c>
+      <c r="W35">
+        <v>0.7</v>
+      </c>
+      <c r="X35" s="5">
+        <f>W35</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5">
+        <f>E36</f>
+        <v>27.8</v>
+      </c>
+      <c r="E36">
+        <v>27.8</v>
+      </c>
+      <c r="H36">
+        <v>22.4</v>
+      </c>
+      <c r="I36" s="5">
+        <f>H36</f>
+        <v>22.4</v>
+      </c>
+      <c r="J36">
+        <v>22.1</v>
+      </c>
+      <c r="L36" s="5">
+        <f>M36</f>
+        <v>12.9</v>
+      </c>
+      <c r="M36">
+        <v>12.9</v>
+      </c>
+      <c r="O36">
+        <v>6.6</v>
+      </c>
+      <c r="Q36">
+        <v>4.8</v>
+      </c>
+      <c r="T36">
+        <v>3.4</v>
+      </c>
+      <c r="U36" s="5">
+        <f>T36</f>
+        <v>3.4</v>
+      </c>
+      <c r="V36" s="5">
+        <f>W36</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="W36">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X36" s="5">
+        <f>W36</f>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>59</v>
+      </c>
+      <c r="D37">
+        <v>50.8</v>
+      </c>
+      <c r="F37">
+        <v>44.3</v>
+      </c>
+      <c r="H37">
+        <v>36.9</v>
+      </c>
+      <c r="I37">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="J37">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="K37">
+        <v>29.8</v>
+      </c>
+      <c r="L37">
+        <v>27.4</v>
+      </c>
+      <c r="M37">
+        <v>22.9</v>
+      </c>
+      <c r="N37">
+        <v>22.5</v>
+      </c>
+      <c r="O37">
+        <v>19.5</v>
+      </c>
+      <c r="P37">
+        <v>18.7</v>
+      </c>
+      <c r="Q37">
+        <v>14.6</v>
+      </c>
+      <c r="R37">
+        <v>15.7</v>
+      </c>
+      <c r="S37">
+        <v>15.1</v>
+      </c>
+      <c r="T37">
+        <v>15.6</v>
+      </c>
+      <c r="U37">
+        <v>13.1</v>
+      </c>
+      <c r="V37">
+        <v>13.2</v>
+      </c>
+      <c r="W37">
+        <v>12.2</v>
+      </c>
+      <c r="X37" s="5">
+        <f>W37</f>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <f>D38</f>
+        <v>88.9</v>
+      </c>
+      <c r="D38">
+        <v>88.9</v>
+      </c>
+      <c r="F38">
+        <v>84.2</v>
+      </c>
+      <c r="H38">
+        <v>79.8</v>
+      </c>
+      <c r="I38" s="5">
+        <f>H38</f>
+        <v>79.8</v>
+      </c>
+      <c r="J38">
+        <v>77.7</v>
+      </c>
+      <c r="L38">
+        <v>46.7</v>
+      </c>
+      <c r="N38">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="P38">
+        <v>34.9</v>
+      </c>
+      <c r="R38">
+        <v>27.1</v>
+      </c>
+      <c r="T38">
+        <v>22.2</v>
+      </c>
+      <c r="U38" s="5">
+        <f>T38</f>
+        <v>22.2</v>
+      </c>
+      <c r="V38">
+        <v>18.7</v>
+      </c>
+      <c r="W38" s="5">
+        <f>V38</f>
+        <v>18.7</v>
+      </c>
+      <c r="X38">
+        <v>19.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23080,10 +25269,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E209C58E-6D7E-40CA-9A2E-E09184173097}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X34" sqref="X34"/>
+    <sheetView topLeftCell="J14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25394,7 +27583,7 @@
         <v>7.5721998214721697</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -25450,7 +27639,7 @@
         <v>2.6143035888671902</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -25522,6 +27711,289 @@
       </c>
       <c r="X34" s="5">
         <v>5.4282999038696298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>4.0182199478149396</v>
+      </c>
+      <c r="C35">
+        <v>4.1001400947570801</v>
+      </c>
+      <c r="D35">
+        <v>4.6119298934936497</v>
+      </c>
+      <c r="E35">
+        <v>4.8012900352478001</v>
+      </c>
+      <c r="F35">
+        <v>4.7355499267578098</v>
+      </c>
+      <c r="G35">
+        <v>4.92976999282837</v>
+      </c>
+      <c r="H35">
+        <v>4.9764900207519496</v>
+      </c>
+      <c r="I35">
+        <v>4.9244499206543004</v>
+      </c>
+      <c r="J35">
+        <v>4.9097399711608896</v>
+      </c>
+      <c r="K35">
+        <v>5.0626301765441903</v>
+      </c>
+      <c r="L35">
+        <v>5.6986799240112296</v>
+      </c>
+      <c r="M35">
+        <v>5.5721898078918501</v>
+      </c>
+      <c r="N35">
+        <v>5.5788741111755398</v>
+      </c>
+      <c r="O35">
+        <v>5.5253000259399396</v>
+      </c>
+      <c r="P35">
+        <v>5.6013498306274396</v>
+      </c>
+      <c r="Q35">
+        <v>5.5545201301574698</v>
+      </c>
+      <c r="R35">
+        <v>5.4279599189758301</v>
+      </c>
+      <c r="S35">
+        <v>5.4525699615478498</v>
+      </c>
+      <c r="T35">
+        <v>5.2043700218200701</v>
+      </c>
+      <c r="U35">
+        <v>5.2611598968505904</v>
+      </c>
+      <c r="V35">
+        <v>5.4393501281738299</v>
+      </c>
+      <c r="W35">
+        <v>5.90458011627197</v>
+      </c>
+      <c r="X35">
+        <v>4.9591755867004403</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>5.9716100692748997</v>
+      </c>
+      <c r="C36">
+        <v>7.4844698905944798</v>
+      </c>
+      <c r="D36">
+        <v>7.6579298973083496</v>
+      </c>
+      <c r="E36">
+        <v>7.5028800964355504</v>
+      </c>
+      <c r="F36">
+        <v>5.92389011383057</v>
+      </c>
+      <c r="H36">
+        <v>4.4857602119445801</v>
+      </c>
+      <c r="I36">
+        <v>4.3725399971008301</v>
+      </c>
+      <c r="J36">
+        <v>3.9585199356079102</v>
+      </c>
+      <c r="K36">
+        <v>5.9741802215576199</v>
+      </c>
+      <c r="L36">
+        <v>4.9664502143859899</v>
+      </c>
+      <c r="M36">
+        <v>5.76293992996216</v>
+      </c>
+      <c r="N36">
+        <v>5.7390298843383798</v>
+      </c>
+      <c r="O36">
+        <v>5.48120021820068</v>
+      </c>
+      <c r="P36">
+        <v>5.0293598175048801</v>
+      </c>
+      <c r="Q36">
+        <v>4.7038102149963397</v>
+      </c>
+      <c r="R36">
+        <v>4.3459844589233398</v>
+      </c>
+      <c r="S36">
+        <v>4.1848850250244096</v>
+      </c>
+      <c r="T36">
+        <v>4.1319484710693404</v>
+      </c>
+      <c r="U36">
+        <v>3.9795396327972399</v>
+      </c>
+      <c r="V36">
+        <v>4.5188870429992702</v>
+      </c>
+      <c r="W36">
+        <v>4.2610940933227504</v>
+      </c>
+      <c r="X36">
+        <v>3.4993379116058301</v>
+      </c>
+      <c r="Y36">
+        <v>3.6272549629211399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>5.2534599304199201</v>
+      </c>
+      <c r="C37">
+        <v>4.81787014007568</v>
+      </c>
+      <c r="D37">
+        <v>3.8649199008941699</v>
+      </c>
+      <c r="E37">
+        <v>3.7256100177764901</v>
+      </c>
+      <c r="F37">
+        <v>4.0308899879455602</v>
+      </c>
+      <c r="G37">
+        <v>3.9385900497436501</v>
+      </c>
+      <c r="H37">
+        <v>4.0503802299499503</v>
+      </c>
+      <c r="I37">
+        <v>3.60314989089966</v>
+      </c>
+      <c r="J37">
+        <v>3.5085000991821298</v>
+      </c>
+      <c r="K37">
+        <v>3.8619399070739702</v>
+      </c>
+      <c r="L37">
+        <v>3.5084400177002002</v>
+      </c>
+      <c r="M37">
+        <v>4.8055500984191903</v>
+      </c>
+      <c r="N37">
+        <v>3.5969183444976802</v>
+      </c>
+      <c r="O37">
+        <v>3.8243985176086399</v>
+      </c>
+      <c r="P37">
+        <v>3.91917753219604</v>
+      </c>
+      <c r="Q37">
+        <v>3.8639762401580802</v>
+      </c>
+      <c r="R37">
+        <v>3.76761746406555</v>
+      </c>
+      <c r="S37">
+        <v>3.46532154083252</v>
+      </c>
+      <c r="T37">
+        <v>3.1976940631866499</v>
+      </c>
+      <c r="U37">
+        <v>3.0222141742706299</v>
+      </c>
+      <c r="V37">
+        <v>3.1531417369842498</v>
+      </c>
+      <c r="W37">
+        <v>2.9821243286132799</v>
+      </c>
+      <c r="X37">
+        <v>2.6118702888488801</v>
+      </c>
+      <c r="Y37">
+        <v>2.5212221145629901</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <f>J38</f>
+        <v>4.88674020767212</v>
+      </c>
+      <c r="I38" s="5">
+        <f>J38</f>
+        <v>4.88674020767212</v>
+      </c>
+      <c r="J38">
+        <v>4.88674020767212</v>
+      </c>
+      <c r="K38">
+        <v>4.8165001869201696</v>
+      </c>
+      <c r="L38">
+        <v>4.0459399223327601</v>
+      </c>
+      <c r="M38">
+        <v>3.7802300453186</v>
+      </c>
+      <c r="N38">
+        <v>4.4081702232360804</v>
+      </c>
+      <c r="O38">
+        <v>4.5283398628234899</v>
+      </c>
+      <c r="P38">
+        <v>3.5401232242584202</v>
+      </c>
+      <c r="Q38">
+        <v>3.41660451889038</v>
+      </c>
+      <c r="R38">
+        <v>3.4690740108489999</v>
+      </c>
+      <c r="S38">
+        <v>3.4186568260192902</v>
+      </c>
+      <c r="T38">
+        <v>3.1450231075286901</v>
+      </c>
+      <c r="U38">
+        <v>3.0849983692169198</v>
+      </c>
+      <c r="V38">
+        <v>3.2165288925170898</v>
+      </c>
+      <c r="W38">
+        <v>2.9451749324798602</v>
+      </c>
+      <c r="X38">
+        <v>2.8873867988586399</v>
       </c>
     </row>
   </sheetData>
@@ -25531,10 +28003,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6C9A80-857C-43F3-9EAD-2E808DECD708}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28122,6 +30594,309 @@
         <v>12</v>
       </c>
     </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>11</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>11</v>
+      </c>
+      <c r="H35">
+        <v>11</v>
+      </c>
+      <c r="I35">
+        <v>11</v>
+      </c>
+      <c r="J35">
+        <v>11</v>
+      </c>
+      <c r="K35">
+        <v>11</v>
+      </c>
+      <c r="L35">
+        <v>11</v>
+      </c>
+      <c r="M35">
+        <v>11</v>
+      </c>
+      <c r="N35">
+        <v>11</v>
+      </c>
+      <c r="O35">
+        <v>11</v>
+      </c>
+      <c r="P35">
+        <v>11</v>
+      </c>
+      <c r="Q35">
+        <v>11</v>
+      </c>
+      <c r="R35">
+        <v>11</v>
+      </c>
+      <c r="S35">
+        <v>11</v>
+      </c>
+      <c r="T35">
+        <v>11</v>
+      </c>
+      <c r="U35">
+        <v>11</v>
+      </c>
+      <c r="V35">
+        <v>11</v>
+      </c>
+      <c r="W35">
+        <v>11</v>
+      </c>
+      <c r="X35">
+        <v>11</v>
+      </c>
+      <c r="Y35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5">
+        <f>E36</f>
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <v>6</v>
+      </c>
+      <c r="K36">
+        <v>6</v>
+      </c>
+      <c r="L36">
+        <v>6</v>
+      </c>
+      <c r="M36">
+        <v>6</v>
+      </c>
+      <c r="N36">
+        <v>6</v>
+      </c>
+      <c r="O36">
+        <v>6</v>
+      </c>
+      <c r="P36">
+        <v>6</v>
+      </c>
+      <c r="Q36">
+        <v>6</v>
+      </c>
+      <c r="R36">
+        <v>6</v>
+      </c>
+      <c r="S36">
+        <v>6</v>
+      </c>
+      <c r="T36">
+        <v>6</v>
+      </c>
+      <c r="U36">
+        <v>6</v>
+      </c>
+      <c r="V36">
+        <v>6</v>
+      </c>
+      <c r="W36">
+        <v>6</v>
+      </c>
+      <c r="X36">
+        <v>6</v>
+      </c>
+      <c r="Y36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <v>9</v>
+      </c>
+      <c r="E37">
+        <v>9</v>
+      </c>
+      <c r="F37">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>9</v>
+      </c>
+      <c r="I37">
+        <v>9</v>
+      </c>
+      <c r="J37">
+        <v>9</v>
+      </c>
+      <c r="K37">
+        <v>9</v>
+      </c>
+      <c r="L37">
+        <v>9</v>
+      </c>
+      <c r="M37">
+        <v>9</v>
+      </c>
+      <c r="N37">
+        <v>9</v>
+      </c>
+      <c r="O37">
+        <v>9</v>
+      </c>
+      <c r="P37">
+        <v>9</v>
+      </c>
+      <c r="Q37">
+        <v>9</v>
+      </c>
+      <c r="R37">
+        <v>9</v>
+      </c>
+      <c r="S37">
+        <v>9</v>
+      </c>
+      <c r="T37">
+        <v>9</v>
+      </c>
+      <c r="U37">
+        <v>9</v>
+      </c>
+      <c r="V37">
+        <v>9</v>
+      </c>
+      <c r="W37">
+        <v>9</v>
+      </c>
+      <c r="X37">
+        <v>9</v>
+      </c>
+      <c r="Y37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <v>9</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38">
+        <v>9</v>
+      </c>
+      <c r="K38">
+        <v>9</v>
+      </c>
+      <c r="L38">
+        <v>9</v>
+      </c>
+      <c r="M38">
+        <v>9</v>
+      </c>
+      <c r="N38">
+        <v>9</v>
+      </c>
+      <c r="O38">
+        <v>9</v>
+      </c>
+      <c r="P38">
+        <v>9</v>
+      </c>
+      <c r="Q38">
+        <v>10</v>
+      </c>
+      <c r="R38">
+        <v>10</v>
+      </c>
+      <c r="S38">
+        <v>10</v>
+      </c>
+      <c r="T38">
+        <v>10</v>
+      </c>
+      <c r="U38">
+        <v>10</v>
+      </c>
+      <c r="V38">
+        <v>10</v>
+      </c>
+      <c r="W38">
+        <v>10</v>
+      </c>
+      <c r="X38">
+        <v>10</v>
+      </c>
+      <c r="Y38">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28129,10 +30904,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC4A6BD7-E576-4656-A9D8-D35416F4A13C}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30350,7 +33125,7 @@
         <v>83.897613525390597</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -30425,7 +33200,7 @@
         <v>127.57797241210901</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -30473,6 +33248,293 @@
       </c>
       <c r="X34">
         <v>79.361930847167997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>57.365119934082003</v>
+      </c>
+      <c r="C35">
+        <v>57.487300872802699</v>
+      </c>
+      <c r="D35">
+        <v>61.128219604492202</v>
+      </c>
+      <c r="E35">
+        <v>61.455970764160199</v>
+      </c>
+      <c r="F35">
+        <v>59.452671051025398</v>
+      </c>
+      <c r="G35">
+        <v>59.274501800537102</v>
+      </c>
+      <c r="H35">
+        <v>59.190719604492202</v>
+      </c>
+      <c r="I35">
+        <v>58.845088958740199</v>
+      </c>
+      <c r="J35">
+        <v>57.430988311767599</v>
+      </c>
+      <c r="K35">
+        <v>59.101131439208999</v>
+      </c>
+      <c r="L35">
+        <v>59.846729278564503</v>
+      </c>
+      <c r="M35">
+        <v>59.3426704406738</v>
+      </c>
+      <c r="N35">
+        <v>59.149940490722699</v>
+      </c>
+      <c r="O35">
+        <v>56.762889862060497</v>
+      </c>
+      <c r="P35">
+        <v>56.487911224365199</v>
+      </c>
+      <c r="Q35">
+        <v>56.397129058837898</v>
+      </c>
+      <c r="R35">
+        <v>58.019100189208999</v>
+      </c>
+      <c r="S35">
+        <v>59.554798126220703</v>
+      </c>
+      <c r="T35">
+        <v>61.091880798339801</v>
+      </c>
+      <c r="U35">
+        <v>65.524940490722699</v>
+      </c>
+      <c r="V35">
+        <v>69.530380249023395</v>
+      </c>
+      <c r="W35">
+        <v>77.076881408691406</v>
+      </c>
+      <c r="X35">
+        <v>80.151100158691406</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>27.015060424804702</v>
+      </c>
+      <c r="C36">
+        <v>26.424640655517599</v>
+      </c>
+      <c r="D36">
+        <v>28.730180740356399</v>
+      </c>
+      <c r="E36">
+        <v>31.4712009429932</v>
+      </c>
+      <c r="F36">
+        <v>30.2977600097656</v>
+      </c>
+      <c r="G36">
+        <v>27.687089920043899</v>
+      </c>
+      <c r="H36">
+        <v>28.2458801269531</v>
+      </c>
+      <c r="I36">
+        <v>29.857660293579102</v>
+      </c>
+      <c r="J36">
+        <v>33.2592582702637</v>
+      </c>
+      <c r="K36">
+        <v>35.237831115722699</v>
+      </c>
+      <c r="L36">
+        <v>36.6847114562988</v>
+      </c>
+      <c r="M36">
+        <v>35.659858703613303</v>
+      </c>
+      <c r="N36">
+        <v>36.9332084655762</v>
+      </c>
+      <c r="O36">
+        <v>38.232719421386697</v>
+      </c>
+      <c r="P36">
+        <v>38.676826477050803</v>
+      </c>
+      <c r="Q36">
+        <v>44.869503021240199</v>
+      </c>
+      <c r="R36">
+        <v>46.401668548583999</v>
+      </c>
+      <c r="S36">
+        <v>43.668045043945298</v>
+      </c>
+      <c r="T36">
+        <v>45.278415679931598</v>
+      </c>
+      <c r="U36">
+        <v>43.197715759277301</v>
+      </c>
+      <c r="V36">
+        <v>42.409767150878899</v>
+      </c>
+      <c r="W36">
+        <v>40.914260864257798</v>
+      </c>
+      <c r="X36">
+        <v>40.270660400390597</v>
+      </c>
+      <c r="Y36">
+        <v>41.261856079101598</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>35.303871154785199</v>
+      </c>
+      <c r="C37">
+        <v>39.0153999328613</v>
+      </c>
+      <c r="D37">
+        <v>40.217559814453097</v>
+      </c>
+      <c r="E37">
+        <v>41.285930633544901</v>
+      </c>
+      <c r="F37">
+        <v>42.313121795654297</v>
+      </c>
+      <c r="G37">
+        <v>44.564468383789098</v>
+      </c>
+      <c r="H37">
+        <v>44.420101165771499</v>
+      </c>
+      <c r="I37">
+        <v>47.754589080810497</v>
+      </c>
+      <c r="J37">
+        <v>46.446701049804702</v>
+      </c>
+      <c r="K37">
+        <v>46.200340270996101</v>
+      </c>
+      <c r="L37">
+        <v>51.239410400390597</v>
+      </c>
+      <c r="M37">
+        <v>52.135963439941399</v>
+      </c>
+      <c r="N37">
+        <v>50.211902618408203</v>
+      </c>
+      <c r="O37">
+        <v>49.334201812744098</v>
+      </c>
+      <c r="P37">
+        <v>49.755733489990199</v>
+      </c>
+      <c r="R37">
+        <v>49.508472442627003</v>
+      </c>
+      <c r="S37">
+        <v>47.722877502441399</v>
+      </c>
+      <c r="T37">
+        <v>46.539951324462898</v>
+      </c>
+      <c r="U37">
+        <v>45.440738677978501</v>
+      </c>
+      <c r="V37">
+        <v>43.114540100097699</v>
+      </c>
+      <c r="W37">
+        <v>44.083087921142599</v>
+      </c>
+      <c r="X37">
+        <v>43.960609436035199</v>
+      </c>
+      <c r="Y37">
+        <v>46.175209045410199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>9.1352500915527308</v>
+      </c>
+      <c r="C38">
+        <v>9.2301797866821307</v>
+      </c>
+      <c r="D38">
+        <v>9.5805702209472692</v>
+      </c>
+      <c r="E38">
+        <v>10.0598201751709</v>
+      </c>
+      <c r="G38">
+        <v>16.332799911498999</v>
+      </c>
+      <c r="H38">
+        <v>17.242010116577099</v>
+      </c>
+      <c r="I38">
+        <v>19.2340602874756</v>
+      </c>
+      <c r="J38">
+        <v>20.0779705047607</v>
+      </c>
+      <c r="K38">
+        <v>21.506200790405298</v>
+      </c>
+      <c r="L38">
+        <v>24.310827255248999</v>
+      </c>
+      <c r="M38">
+        <v>26.618211746215799</v>
+      </c>
+      <c r="N38">
+        <v>26.909589767456101</v>
+      </c>
+      <c r="O38">
+        <v>26.940311431884801</v>
+      </c>
+      <c r="P38">
+        <v>32.865993499755902</v>
+      </c>
+      <c r="Q38">
+        <v>31.089204788208001</v>
+      </c>
+      <c r="R38">
+        <v>30.228063583373999</v>
+      </c>
+      <c r="U38">
+        <v>28.506929397583001</v>
+      </c>
+      <c r="W38">
+        <v>38.873237609863303</v>
+      </c>
+      <c r="X38">
+        <v>42.224239349365199</v>
       </c>
     </row>
   </sheetData>
@@ -30482,10 +33544,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C96331-F4CE-4632-9B42-50E8B8786068}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+    <sheetView topLeftCell="G18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32717,7 +35779,7 @@
         <v>108.32688140869099</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -32792,7 +35854,7 @@
         <v>130.03057861328099</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -32840,6 +35902,295 @@
       </c>
       <c r="X34">
         <v>94.8502197265625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>62.237628936767599</v>
+      </c>
+      <c r="C35">
+        <v>63.150611877441399</v>
+      </c>
+      <c r="D35">
+        <v>68.133651733398395</v>
+      </c>
+      <c r="E35">
+        <v>69.476028442382798</v>
+      </c>
+      <c r="F35">
+        <v>68.748092651367202</v>
+      </c>
+      <c r="G35">
+        <v>68.641181945800795</v>
+      </c>
+      <c r="H35">
+        <v>68.456626892089801</v>
+      </c>
+      <c r="I35">
+        <v>67.892158508300795</v>
+      </c>
+      <c r="J35">
+        <v>66.161231994628906</v>
+      </c>
+      <c r="K35">
+        <v>67.7098388671875</v>
+      </c>
+      <c r="L35">
+        <v>68.325912475585895</v>
+      </c>
+      <c r="M35">
+        <v>67.869102478027301</v>
+      </c>
+      <c r="N35">
+        <v>67.677520751953097</v>
+      </c>
+      <c r="O35">
+        <v>64.673362731933594</v>
+      </c>
+      <c r="P35">
+        <v>64.226287841796903</v>
+      </c>
+      <c r="Q35">
+        <v>64.431457519531193</v>
+      </c>
+      <c r="R35">
+        <v>66.606277465820298</v>
+      </c>
+      <c r="S35">
+        <v>68.663040161132798</v>
+      </c>
+      <c r="T35">
+        <v>70.522682189941406</v>
+      </c>
+      <c r="U35">
+        <v>75.575927734375</v>
+      </c>
+      <c r="V35">
+        <v>79.819931030273395</v>
+      </c>
+      <c r="W35">
+        <v>88.932403564453097</v>
+      </c>
+      <c r="X35">
+        <v>92.98046875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>28.121160507202099</v>
+      </c>
+      <c r="C36">
+        <v>29.4617595672607</v>
+      </c>
+      <c r="D36">
+        <v>32.681278228759801</v>
+      </c>
+      <c r="E36">
+        <v>37.375160217285199</v>
+      </c>
+      <c r="F36">
+        <v>34.935760498046903</v>
+      </c>
+      <c r="G36">
+        <v>32.326080322265597</v>
+      </c>
+      <c r="H36">
+        <v>32.270351409912102</v>
+      </c>
+      <c r="I36">
+        <v>34.658451080322301</v>
+      </c>
+      <c r="J36">
+        <v>38.519779205322301</v>
+      </c>
+      <c r="K36">
+        <v>40.544601440429702</v>
+      </c>
+      <c r="L36">
+        <v>42.7966117858887</v>
+      </c>
+      <c r="M36">
+        <v>40.9309692382812</v>
+      </c>
+      <c r="N36">
+        <v>42.520927429199197</v>
+      </c>
+      <c r="O36">
+        <v>44.250308990478501</v>
+      </c>
+      <c r="P36">
+        <v>44.481452941894503</v>
+      </c>
+      <c r="Q36">
+        <v>50.836158752441399</v>
+      </c>
+      <c r="R36">
+        <v>50.158336639404297</v>
+      </c>
+      <c r="S36">
+        <v>46.950553894042997</v>
+      </c>
+      <c r="T36">
+        <v>49.908454895019503</v>
+      </c>
+      <c r="U36">
+        <v>48.775733947753899</v>
+      </c>
+      <c r="V36">
+        <v>48.162281036377003</v>
+      </c>
+      <c r="W36">
+        <v>46.665908813476598</v>
+      </c>
+      <c r="X36">
+        <v>46.106544494628899</v>
+      </c>
+      <c r="Y36">
+        <v>47.7291069030762</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>38.7144584655762</v>
+      </c>
+      <c r="C37">
+        <v>41.658981323242202</v>
+      </c>
+      <c r="D37">
+        <v>42.519218444824197</v>
+      </c>
+      <c r="E37">
+        <v>44.403400421142599</v>
+      </c>
+      <c r="F37">
+        <v>46.204948425292997</v>
+      </c>
+      <c r="G37">
+        <v>47.571121215820298</v>
+      </c>
+      <c r="H37">
+        <v>46.265769958496101</v>
+      </c>
+      <c r="I37">
+        <v>53.146930694580099</v>
+      </c>
+      <c r="J37">
+        <v>51.240070343017599</v>
+      </c>
+      <c r="K37">
+        <v>51.292018890380902</v>
+      </c>
+      <c r="L37">
+        <v>57.401821136474602</v>
+      </c>
+      <c r="M37">
+        <v>58.360160827636697</v>
+      </c>
+      <c r="N37">
+        <v>56.974124908447301</v>
+      </c>
+      <c r="O37">
+        <v>56.658618927002003</v>
+      </c>
+      <c r="P37">
+        <v>57.050971984863303</v>
+      </c>
+      <c r="R37">
+        <v>57.701000213622997</v>
+      </c>
+      <c r="S37">
+        <v>55.478553771972699</v>
+      </c>
+      <c r="T37">
+        <v>54.472053527832003</v>
+      </c>
+      <c r="U37">
+        <v>52.682132720947301</v>
+      </c>
+      <c r="V37">
+        <v>49.892730712890597</v>
+      </c>
+      <c r="W37">
+        <v>50.666568756103501</v>
+      </c>
+      <c r="X37">
+        <v>50.4828491210938</v>
+      </c>
+      <c r="Y37">
+        <v>53.118881225585902</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>7.6971898078918501</v>
+      </c>
+      <c r="C38">
+        <v>7.8454399108886701</v>
+      </c>
+      <c r="D38">
+        <v>8.2687301635742205</v>
+      </c>
+      <c r="E38">
+        <v>8.7015199661254901</v>
+      </c>
+      <c r="G38">
+        <v>13.387490272521999</v>
+      </c>
+      <c r="H38">
+        <v>16.6284694671631</v>
+      </c>
+      <c r="I38">
+        <v>18.9481601715088</v>
+      </c>
+      <c r="J38">
+        <v>19.550279617309599</v>
+      </c>
+      <c r="K38">
+        <v>21.039659500122099</v>
+      </c>
+      <c r="L38">
+        <v>23.917955398559599</v>
+      </c>
+      <c r="M38">
+        <v>26.3632717132568</v>
+      </c>
+      <c r="O38">
+        <v>25.1871032714844</v>
+      </c>
+      <c r="P38">
+        <v>33.294715881347699</v>
+      </c>
+      <c r="Q38">
+        <v>30.792671203613299</v>
+      </c>
+      <c r="R38">
+        <v>33.217681884765597</v>
+      </c>
+      <c r="U38" s="5">
+        <f>R38</f>
+        <v>33.217681884765597</v>
+      </c>
+      <c r="V38" s="5">
+        <f>W38</f>
+        <v>38.618888854980497</v>
+      </c>
+      <c r="W38">
+        <v>38.618888854980497</v>
+      </c>
+      <c r="X38">
+        <v>43.58251953125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>